<commit_message>
EAS and MTS - Checklist
</commit_message>
<xml_diff>
--- a/hcsa-licence-be/src/main/resources/template/Checklist_Config_Update_Template.xlsx
+++ b/hcsa-licence-be/src/main/resources/template/Checklist_Config_Update_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\iais-egp-sz\hcsa-licence-be\src\main\resources\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IDE\IdeaProjects\moh_iais\iais-egp\hcsa-licence-be\src\main\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1304989-E3F8-4D37-AABF-E52F5F1EFA28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCA14FD-4FB4-4DD4-88EA-D0E772824765}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -30,14 +30,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -47,7 +47,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -57,7 +57,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -70,7 +70,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -80,7 +80,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -90,7 +90,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -103,7 +103,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -113,7 +113,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -123,7 +123,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -178,7 +178,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -188,7 +188,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -213,7 +213,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -223,7 +223,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -239,7 +239,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -250,7 +250,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -260,7 +260,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -273,7 +273,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -284,7 +284,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -294,7 +294,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -307,7 +307,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -318,7 +318,7 @@
         <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -328,7 +328,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="等线"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -388,24 +388,27 @@
   <si>
     <t>Next Config Id</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inspection Entity:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -413,7 +416,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -421,7 +424,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -430,13 +433,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -474,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -493,12 +496,85 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -518,7 +594,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CEEACA"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -779,18 +855,18 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="63.75" customWidth="1"/>
+    <col min="2" max="2" width="63.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="3"/>
       <c r="B1" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="30">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -798,7 +874,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="30">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -806,7 +882,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="45">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -814,7 +890,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="30">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -822,7 +898,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="30">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -830,7 +906,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="45">
       <c r="A7" s="6">
         <v>5</v>
       </c>
@@ -847,45 +923,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="33.25" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
-    <col min="4" max="4" width="21.375" customWidth="1"/>
-    <col min="5" max="5" width="19.75" customWidth="1"/>
-    <col min="6" max="6" width="16.375" customWidth="1"/>
-    <col min="7" max="7" width="18.875" customWidth="1"/>
-    <col min="8" max="8" width="15.625" customWidth="1"/>
-    <col min="11" max="11" width="13.625" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="P1" s="1" t="s">
+    <row r="1" spans="1:20">
+      <c r="P1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S1" s="9"/>
+      <c r="T1" s="10"/>
+    </row>
+    <row r="2" spans="1:20">
       <c r="B2" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+    </row>
+    <row r="4" spans="1:20">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -899,7 +983,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -910,8 +994,12 @@
         <v>17</v>
       </c>
       <c r="F6" s="4"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="H6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="8" spans="1:20">
       <c r="B8" t="s">
         <v>22</v>
       </c>
@@ -922,14 +1010,14 @@
       <c r="F8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="I8" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -981,77 +1069,77 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="22.75" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:2">
       <c r="B1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2">
       <c r="B2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2">
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2">
       <c r="B4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:2">
       <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:2">
       <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:2">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:2">
       <c r="B11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:2">
       <c r="B12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:2">
       <c r="B13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:2">
       <c r="B14" t="s">
         <v>14</v>
       </c>

</xml_diff>